<commit_message>
Added verifications and dataprovider for the first test
</commit_message>
<xml_diff>
--- a/src/test/resources/data/OpenCartData.xlsx
+++ b/src/test/resources/data/OpenCartData.xlsx
@@ -21,78 +21,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>TestCases</t>
   </si>
   <si>
-    <t>URL</t>
-  </si>
-  <si>
     <t>Browser</t>
   </si>
   <si>
     <t>Chrome</t>
   </si>
   <si>
-    <t>https://www.linkedin.com</t>
-  </si>
-  <si>
-    <t>FirstName</t>
-  </si>
-  <si>
-    <t>LastName</t>
-  </si>
-  <si>
-    <t>City</t>
-  </si>
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>Phone</t>
-  </si>
-  <si>
-    <t>Sam</t>
-  </si>
-  <si>
-    <t>Smith</t>
-  </si>
-  <si>
-    <t>Pune</t>
-  </si>
-  <si>
-    <t>India</t>
-  </si>
-  <si>
     <t xml:space="preserve">  </t>
   </si>
   <si>
-    <t>https://stackoverflow.com</t>
-  </si>
-  <si>
-    <t>Richard</t>
-  </si>
-  <si>
-    <t>Kane</t>
-  </si>
-  <si>
-    <t>Perth</t>
-  </si>
-  <si>
-    <t>Australia</t>
-  </si>
-  <si>
-    <t>opencartTest1</t>
-  </si>
-  <si>
-    <t>opencartTest2</t>
-  </si>
-  <si>
-    <t>opencartTest3</t>
-  </si>
-  <si>
     <t>http://opencart.abstracta.us/</t>
+  </si>
+  <si>
+    <t>validateProductSearch</t>
+  </si>
+  <si>
+    <t>url</t>
   </si>
 </sst>
 </file>
@@ -108,15 +57,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -124,13 +79,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -411,10 +383,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -424,105 +396,50 @@
     <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3">
-        <v>1234</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4">
-        <v>2222</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>

</xml_diff>